<commit_message>
Commit contains: 1. complete code for project workbook 2. comments in html files for pragun to code.
</commit_message>
<xml_diff>
--- a/src/main/java/corecentra/qaqctool/storage/lookupfile_test.xlsx
+++ b/src/main/java/corecentra/qaqctool/storage/lookupfile_test.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MS\3_Spring2022\5500\old project\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MS\3_Spring2022\5500\qaqctool\src\main\java\corecentra\qaqctool\storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{803A31EA-7A6F-4E8C-898D-C5D65E2BB8B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE6F300D-83DA-47F7-B4C8-6F1A19EB3407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" tabRatio="716" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="695" yWindow="695" windowWidth="14400" windowHeight="7380" tabRatio="716" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Project" sheetId="9" r:id="rId1"/>
+    <sheet name="Projects" sheetId="9" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="10" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -218,10 +218,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,7 +443,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.40625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.75"/>
@@ -551,37 +551,37 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.75">
       <c r="A1" s="4"/>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
       <c r="F1" s="4"/>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
       <c r="K1" s="4"/>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
       <c r="P1" s="4"/>
-      <c r="Q1" s="7" t="s">
+      <c r="Q1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="R1" s="6"/>
+      <c r="R1" s="7"/>
       <c r="S1" s="4"/>
-      <c r="T1" s="7" t="s">
+      <c r="T1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
     </row>
     <row r="2" spans="1:22" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A2" s="5"/>

</xml_diff>

<commit_message>
completed MVC for task file checker.
</commit_message>
<xml_diff>
--- a/src/main/java/corecentra/qaqctool/storage/lookupfile_test.xlsx
+++ b/src/main/java/corecentra/qaqctool/storage/lookupfile_test.xlsx
@@ -8,20 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MS\3_Spring2022\5500\qaqctool\src\main\java\corecentra\qaqctool\storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE6F300D-83DA-47F7-B4C8-6F1A19EB3407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5772EA89-6C6B-41D4-9A48-00AFA261F4D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="695" yWindow="695" windowWidth="14400" windowHeight="7380" tabRatio="716" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" tabRatio="716" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="9" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="10" r:id="rId2"/>
+    <sheet name="Results" sheetId="10" r:id="rId2"/>
+    <sheet name="Impacts" sheetId="11" r:id="rId3"/>
+    <sheet name="Tasks" sheetId="12" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="13" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
   <si>
     <t>Node ID</t>
   </si>
@@ -68,15 +71,6 @@
     <t>Result</t>
   </si>
   <si>
-    <t>RESULT</t>
-  </si>
-  <si>
-    <t>IMPACT</t>
-  </si>
-  <si>
-    <t>TASK</t>
-  </si>
-  <si>
     <t>DONORS</t>
   </si>
   <si>
@@ -123,13 +117,34 @@
   </si>
   <si>
     <t>test project 3</t>
+  </si>
+  <si>
+    <t>PRJ0001</t>
+  </si>
+  <si>
+    <t>Clean Water Distribution</t>
+  </si>
+  <si>
+    <t>RS0001</t>
+  </si>
+  <si>
+    <t>Gallons of water distributed</t>
+  </si>
+  <si>
+    <t>IM0001</t>
+  </si>
+  <si>
+    <t>Number of families with access to purified water</t>
+  </si>
+  <si>
+    <t>Contact Jeff at Clean Water Inc for pricing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -140,16 +155,26 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -201,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -215,8 +240,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -442,8 +470,8 @@
   </sheetPr>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.40625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.75"/>
@@ -496,10 +524,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A3" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>8</v>
@@ -508,7 +536,7 @@
         <v>9</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>12</v>
@@ -516,10 +544,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A4" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
@@ -528,10 +556,10 @@
         <v>9</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -541,111 +569,187 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02C9163A-5DD9-4999-A6CC-59CEA298262A}">
-  <dimension ref="A1:V2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:V1048576"/>
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="8.6796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" customWidth="1"/>
+    <col min="4" max="4" width="16.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="59" x14ac:dyDescent="0.75">
+      <c r="A2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8C2726E-76CA-4538-836D-F73D5F21B14C}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="4" max="4" width="35.58984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="59" x14ac:dyDescent="0.75">
+      <c r="A2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C74FD64A-D7A8-4E24-ADDF-753AF3B78E3A}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="3" max="3" width="21.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="88.5" x14ac:dyDescent="0.75">
+      <c r="A2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51524885-1650-4D28-8C6B-012077E74A2C}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A1" s="4"/>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="6" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="R1" s="7"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
-    </row>
-    <row r="2" spans="1:22" ht="29.5" x14ac:dyDescent="0.75">
-      <c r="A2" s="5"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+    </row>
+    <row r="2" spans="1:7" ht="29.5" x14ac:dyDescent="0.75">
       <c r="B2" s="3" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="G2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="5"/>
-      <c r="L2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Q2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>26</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="T1:V1"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="L1:O1"/>
-    <mergeCell ref="Q1:R1"/>
+  <mergeCells count="2">
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="B1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
completed MVC for contribution file checker.
</commit_message>
<xml_diff>
--- a/src/main/java/corecentra/qaqctool/storage/lookupfile_test.xlsx
+++ b/src/main/java/corecentra/qaqctool/storage/lookupfile_test.xlsx
@@ -8,23 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MS\3_Spring2022\5500\qaqctool\src\main\java\corecentra\qaqctool\storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5772EA89-6C6B-41D4-9A48-00AFA261F4D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A372520-7528-474B-B727-3177105DF68E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" tabRatio="716" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" tabRatio="716" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="9" r:id="rId1"/>
     <sheet name="Results" sheetId="10" r:id="rId2"/>
     <sheet name="Impacts" sheetId="11" r:id="rId3"/>
     <sheet name="Tasks" sheetId="12" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="13" r:id="rId5"/>
+    <sheet name="Donors" sheetId="13" r:id="rId5"/>
+    <sheet name="Donor Contribution" sheetId="14" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
   <si>
     <t>Node ID</t>
   </si>
@@ -71,12 +72,6 @@
     <t>Result</t>
   </si>
   <si>
-    <t>DONORS</t>
-  </si>
-  <si>
-    <t>CONTRIBUTIONS</t>
-  </si>
-  <si>
     <t>Impact ID</t>
   </si>
   <si>
@@ -138,13 +133,22 @@
   </si>
   <si>
     <t>Contact Jeff at Clean Water Inc for pricing</t>
+  </si>
+  <si>
+    <t>DNR0000001</t>
+  </si>
+  <si>
+    <t>Gates Foundation</t>
+  </si>
+  <si>
+    <t>43</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -162,13 +166,6 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -226,7 +223,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -237,19 +234,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -524,10 +514,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>8</v>
@@ -536,7 +526,7 @@
         <v>9</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>12</v>
@@ -544,10 +534,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A4" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
@@ -556,10 +546,10 @@
         <v>9</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -597,17 +587,17 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="59" x14ac:dyDescent="0.75">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -637,24 +627,24 @@
         <v>5</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="59" x14ac:dyDescent="0.75">
-      <c r="A2" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>36</v>
+      <c r="A2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -666,8 +656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C74FD64A-D7A8-4E24-ADDF-753AF3B78E3A}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -683,22 +673,22 @@
         <v>5</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="88.5" x14ac:dyDescent="0.75">
-      <c r="A2" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6" t="s">
-        <v>37</v>
+      <c r="A2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -708,49 +698,60 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51524885-1650-4D28-8C6B-012077E74A2C}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G1048576"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A1" s="4"/>
-      <c r="B1" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-    </row>
-    <row r="2" spans="1:7" ht="29.5" x14ac:dyDescent="0.75">
-      <c r="B2" s="3" t="s">
+    <row r="1" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A98F0E8A-06AD-42B4-BD4B-D23B4750FBDF}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>23</v>
+    </row>
+    <row r="2" spans="1:3" ht="44.25" x14ac:dyDescent="0.75">
+      <c r="A2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="B1:C1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>